<commit_message>
Add circle performance comparison.
</commit_message>
<xml_diff>
--- a/progression_images/circle_performance_comparison.xlsx
+++ b/progression_images/circle_performance_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aking\Documents\Alex\Work\CompSci\CS4098\brio-project\progression_images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A13225B-4734-44B8-A4DC-5EF526DCB770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC6FAA-1C0F-4BF1-ADED-B150F6D8C788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{73B61109-674B-4C0C-A8E4-0DBF36CF5418}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>